<commit_message>
NMDS plots updated and all files work with NBC_Figrues.  Added csv export for tables 1 and 2
</commit_message>
<xml_diff>
--- a/permanova.table.xlsx
+++ b/permanova.table.xlsx
@@ -136,19 +136,19 @@
         <v>4.0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.20618638004217674</v>
+        <v>0.2061863800421767</v>
       </c>
       <c r="E2" t="n">
-        <v>0.051546595010544184</v>
+        <v>0.05154659501054418</v>
       </c>
       <c r="F2" t="n">
-        <v>3.0502460788998027</v>
+        <v>3.0502460788998023</v>
       </c>
       <c r="G2" t="n">
-        <v>0.11023002710645899</v>
+        <v>0.11023002710645897</v>
       </c>
       <c r="H2" t="n">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="3">
@@ -162,16 +162,16 @@
         <v>3.0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.805040895458882</v>
+        <v>0.8050408954588818</v>
       </c>
       <c r="E3" t="n">
-        <v>0.2683469651529607</v>
+        <v>0.2683469651529606</v>
       </c>
       <c r="F3" t="n">
-        <v>15.879308382542941</v>
+        <v>15.879308382542934</v>
       </c>
       <c r="G3" t="n">
-        <v>0.43038574958291775</v>
+        <v>0.43038574958291764</v>
       </c>
       <c r="H3" t="n">
         <v>0.001</v>
@@ -188,19 +188,19 @@
         <v>12.0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.18331645360090443</v>
+        <v>0.18331645360090465</v>
       </c>
       <c r="E4" t="n">
-        <v>0.015276371133408703</v>
+        <v>0.01527637113340872</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9039722437527907</v>
+        <v>0.9039722437527917</v>
       </c>
       <c r="G4" t="n">
-        <v>0.09800345515234402</v>
+        <v>0.09800345515234414</v>
       </c>
       <c r="H4" t="n">
-        <v>0.657</v>
+        <v>0.656</v>
       </c>
     </row>
   </sheetData>

</xml_diff>